<commit_message>
feat: Add Data Loader, Json (일반형 몬스터)
</commit_message>
<xml_diff>
--- a/INFEST_Project/Util/ExcelToJsonWizard.v1.0.6/excel_files/CommonSkillTable.xlsx
+++ b/INFEST_Project/Util/ExcelToJsonWizard.v1.0.6/excel_files/CommonSkillTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\worni\Desktop\GitProject\INFEST\INFEST_Project\Util\ExcelToJsonWizard.v1.0.6\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28E9E2C-4699-4869-9817-ADAA6A82BF6C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4D3028-ECA9-4FED-A6C3-5FC8BE59764B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17025" windowHeight="7875" xr2:uid="{CF8620D6-7292-4E8C-8303-344569A6BA25}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>key</t>
   </si>
@@ -45,10 +45,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>SkillPriority</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>int</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -79,19 +75,39 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>사용 우선순위</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>VomitLaser</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>AcidVomit</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Swip</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HeadButt</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DropKick</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Skill_ID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>스킬식별자</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKL_SWIP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKL_HEADBUTT</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKL_DROPKICK</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -483,16 +499,16 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="A1:G7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -500,59 +516,59 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -560,19 +576,19 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4">
         <v>1</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
       <c r="E4">
+        <v>0.5</v>
+      </c>
+      <c r="F4">
         <v>1</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -580,19 +596,19 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5">
-        <v>1.2</v>
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
       </c>
       <c r="D5">
-        <v>7</v>
+        <v>1.3</v>
       </c>
       <c r="E5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -600,23 +616,24 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6">
-        <v>1.5</v>
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
       </c>
       <c r="D6">
-        <v>10</v>
+        <v>1.6</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>